<commit_message>
add experiments with nf
</commit_message>
<xml_diff>
--- a/PAPER_METEO/results.xlsx
+++ b/PAPER_METEO/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">YEAR</t>
   </si>
@@ -59,10 +59,7 @@
     <t xml:space="preserve">FOLD</t>
   </si>
   <si>
-    <t xml:space="preserve">3 features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
+    <t xml:space="preserve">1f</t>
   </si>
 </sst>
 </file>
@@ -178,7 +175,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,6 +220,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,8 +255,8 @@
   </sheetPr>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,12 +322,14 @@
         <v>0.155</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>0.0895</v>
+        <v>0.0836</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>0.0804</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="n">
+        <v>0.0795</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -348,12 +351,14 @@
         <v>0.1503</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>0.0832</v>
+        <v>0.081</v>
       </c>
       <c r="H3" s="4" t="n">
         <v>0.0751</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="n">
+        <v>0.0724</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -375,12 +380,14 @@
         <v>0.1293</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>0.0916</v>
+        <v>0.0861</v>
       </c>
       <c r="H4" s="4" t="n">
         <v>0.086</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="n">
+        <v>0.0815</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -402,12 +409,14 @@
         <v>0.1264</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>0.1265</v>
+        <v>0.1268</v>
       </c>
       <c r="H5" s="4" t="n">
         <v>0.1266</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="n">
+        <v>0.1246</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -429,12 +438,14 @@
         <v>0.1049</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>0.0805</v>
+        <v>0.0768</v>
       </c>
       <c r="H6" s="4" t="n">
         <v>0.0772</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="n">
+        <v>0.0751</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -456,12 +467,14 @@
         <v>0.0972</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>0.0665</v>
+        <v>0.0677</v>
       </c>
       <c r="H7" s="4" t="n">
         <v>0.0662</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="n">
+        <v>0.0649</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -483,12 +496,14 @@
         <v>0.0976</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>0.0952</v>
+        <v>0.095</v>
       </c>
       <c r="H8" s="4" t="n">
         <v>0.0961</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="n">
+        <v>0.0958</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -510,12 +525,14 @@
         <v>0.1103</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>0.1091</v>
+        <v>0.1053</v>
       </c>
       <c r="H9" s="4" t="n">
         <v>0.0955</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="n">
+        <v>0.0962</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
@@ -543,15 +560,15 @@
       </c>
       <c r="G10" s="7" t="n">
         <f aca="false">AVERAGE(G2:G9)</f>
-        <v>0.0927625</v>
+        <v>0.0902875</v>
       </c>
       <c r="H10" s="7" t="n">
         <f aca="false">AVERAGE(H2:H9)</f>
         <v>0.0878875</v>
       </c>
-      <c r="I10" s="7" t="e">
+      <c r="I10" s="7" t="n">
         <f aca="false">AVERAGE(I2:I9)</f>
-        <v>#DIV/0!</v>
+        <v>0.08625</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -692,10 +709,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -704,706 +721,780 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="n">
-        <v>2014</v>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>2015</v>
-      </c>
-      <c r="D1" s="2" t="n">
-        <v>2016</v>
-      </c>
-      <c r="E1" s="2" t="n">
-        <v>2017</v>
-      </c>
-      <c r="F1" s="2" t="n">
-        <v>2018</v>
-      </c>
-      <c r="G1" s="2" t="n">
-        <v>2019</v>
-      </c>
-      <c r="H1" s="2" t="n">
-        <v>2020</v>
-      </c>
-      <c r="I1" s="2" t="n">
-        <v>2021</v>
-      </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>2021</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>0.083</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>0.0707</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>0.0987</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>0.1133</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>0.0812</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>0.0801</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>0.1057</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>0.0889</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="B3" s="4" t="n">
-        <v>0.0919</v>
+        <v>0.0841</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>0.0718</v>
+        <v>0.0783</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>0.1019</v>
+        <v>0.0985</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>0.12</v>
+        <v>0.1131</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>0.0774</v>
+        <v>0.0822</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>0.0687</v>
+        <v>0.0777</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>0.0916</v>
+        <v>0.106</v>
       </c>
       <c r="I3" s="4" t="n">
-        <v>0.1099</v>
-      </c>
+        <v>0.0921</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0.0798</v>
+        <v>0.1053</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0.0838</v>
+        <v>0.0756</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.0903</v>
+        <v>0.1057</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.1226</v>
+        <v>0.1202</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>0.0754</v>
+        <v>0.0797</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>0.0748</v>
+        <v>0.0712</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>0.0999</v>
+        <v>0.0915</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>0.1</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>0.081</v>
+        <v>0.0935</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>0.0829</v>
+        <v>0.083</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.0775</v>
+        <v>0.0916</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.1372</v>
+        <v>0.1224</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>0.0806</v>
+        <v>0.0773</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>0.0548</v>
+        <v>0.076</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>0.1013</v>
+        <v>0.1001</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>0.1026</v>
+        <v>0.0994</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>0.091</v>
+        <v>0.0907</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>0.0773</v>
+        <v>0.089</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>0.085</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>0.1235</v>
+        <v>0.1378</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>0.0702</v>
+        <v>0.0843</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>0.0595</v>
+        <v>0.0555</v>
       </c>
       <c r="H6" s="4" t="n">
-        <v>0.0999</v>
+        <v>0.1012</v>
       </c>
       <c r="I6" s="4" t="n">
-        <v>0.1076</v>
+        <v>0.1044</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.1038</v>
+        <v>0.0884</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>0.0852</v>
+        <v>0.076</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>0.0909</v>
+        <v>0.0882</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>0.1265</v>
+        <v>0.1234</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>0.0823</v>
+        <v>0.0742</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>0.0782</v>
+        <v>0.0577</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>0.0849</v>
+        <v>0.1001</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>0.1125</v>
+        <v>0.1137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>0.0961</v>
+        <v>0.1037</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>0.0881</v>
+        <v>0.0886</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>0.0738</v>
+        <v>0.0883</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>0.1403</v>
+        <v>0.1266</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>0.083</v>
+        <v>0.0816</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>0.0702</v>
+        <v>0.0791</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>0.1015</v>
+        <v>0.0846</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>0.1078</v>
+        <v>0.1097</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>0.1017</v>
+        <v>0.0928</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>0.0854</v>
+        <v>0.0881</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>0.1066</v>
+        <v>0.077</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>0.1297</v>
+        <v>0.1401</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>0.0847</v>
+        <v>0.0857</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>0.054</v>
+        <v>0.0778</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>0.0975</v>
+        <v>0.1018</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>0.1306</v>
+        <v>0.1161</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>0.0902</v>
+        <v>0.1012</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>0.0889</v>
+        <v>0.0862</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>0.1032</v>
+        <v>0.0993</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>0.1315</v>
+        <v>0.1286</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0.0847</v>
+        <v>0.0884</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>0.054</v>
+        <v>0.0596</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>0.0875</v>
+        <v>0.0974</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>0.1306</v>
+        <v>0.1271</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>0.0813</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>0.0898</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>0.1056</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0.1316</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>0.0816</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>0.0714</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>0.0875</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <v>0.1131</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>0.0768</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>0.0976</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>0.0878</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>0.1208</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <v>0.0854</v>
-      </c>
-      <c r="G11" s="4" t="n">
-        <v>0.0705</v>
-      </c>
-      <c r="H11" s="4" t="n">
-        <v>0.0821</v>
-      </c>
-      <c r="I11" s="4" t="n">
-        <v>0.1007</v>
-      </c>
-    </row>
-    <row r="12" s="8" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="n">
-        <f aca="false">AVERAGE(B2:B11)</f>
-        <v>0.08953</v>
-      </c>
-      <c r="C12" s="7" t="n">
-        <f aca="false">AVERAGE(C2:C11)</f>
-        <v>0.08317</v>
-      </c>
-      <c r="D12" s="7" t="n">
-        <f aca="false">AVERAGE(D2:D11)</f>
-        <v>0.09157</v>
-      </c>
-      <c r="E12" s="7" t="n">
-        <f aca="false">AVERAGE(E2:E11)</f>
-        <v>0.12654</v>
-      </c>
-      <c r="F12" s="7" t="n">
-        <f aca="false">AVERAGE(F2:F11)</f>
-        <v>0.08049</v>
-      </c>
-      <c r="G12" s="7" t="n">
-        <f aca="false">AVERAGE(G2:G11)</f>
-        <v>0.06648</v>
-      </c>
-      <c r="H12" s="7" t="n">
-        <f aca="false">AVERAGE(H2:H11)</f>
-        <v>0.09519</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <f aca="false">AVERAGE(I2:I11)</f>
-        <v>0.10912</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="12" t="n">
-        <f aca="false">AVERAGE(B12:I12)</f>
-        <v>0.09276125</v>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="13" t="s">
+      <c r="B12" s="4" t="n">
+        <v>0.0743</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>0.0982</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>0.0894</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0.1203</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>0.0883</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>0.0818</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <v>0.1027</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7" t="n">
+        <f aca="false">AVERAGE(B3:B12)</f>
+        <v>0.09153</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <f aca="false">AVERAGE(C3:C12)</f>
+        <v>0.08528</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <f aca="false">AVERAGE(D3:D12)</f>
+        <v>0.09286</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <f aca="false">AVERAGE(E3:E12)</f>
+        <v>0.12641</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <f aca="false">AVERAGE(F3:F12)</f>
+        <v>0.08233</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <f aca="false">AVERAGE(G3:G12)</f>
+        <v>0.0702</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <f aca="false">AVERAGE(H3:H12)</f>
+        <v>0.0952</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <f aca="false">AVERAGE(I3:I12)</f>
+        <v>0.10903</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="13" t="n">
+        <f aca="false">AVERAGE(B13:I13)</f>
+        <v>0.094105</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B16" s="2" t="n">
         <v>2014</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C16" s="2" t="n">
         <v>2015</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D16" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E16" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F16" s="2" t="n">
         <v>2018</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G16" s="2" t="n">
         <v>2019</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H16" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="I16" s="2" t="n">
         <v>2021</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>0.077</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>0.0714</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>0.0925</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v>0.1132</v>
-      </c>
-      <c r="F16" s="4" t="n">
-        <v>0.0771</v>
-      </c>
-      <c r="G16" s="4" t="n">
-        <v>0.0785</v>
-      </c>
-      <c r="H16" s="4" t="n">
-        <v>0.1055</v>
-      </c>
-      <c r="I16" s="4" t="n">
-        <v>0.0833</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="4" t="n">
-        <v>0.0971</v>
+        <v>0.0775</v>
       </c>
       <c r="C17" s="4" t="n">
-        <v>0.0701</v>
+        <v>0.0649</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>0.0954</v>
+        <v>0.0868</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>0.1204</v>
+        <v>0.1138</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>0.0742</v>
+        <v>0.0657</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>0.0644</v>
+        <v>0.0754</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>0.0923</v>
+        <v>0.1075</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>0.1034</v>
+        <v>0.0817</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="4" t="n">
-        <v>0.0761</v>
+        <v>0.0826</v>
       </c>
       <c r="C18" s="4" t="n">
-        <v>0.0758</v>
+        <v>0.062</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>0.0828</v>
+        <v>0.095</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>0.123</v>
+        <v>0.1204</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>0.0732</v>
+        <v>0.064</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>0.0722</v>
+        <v>0.0737</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>0.1003</v>
+        <v>0.0959</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>0.0899</v>
+        <v>0.1013</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="4" t="n">
-        <v>0.0785</v>
+        <v>0.0735</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>0.0712</v>
+        <v>0.0786</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>0.0826</v>
+        <v>0.0735</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>0.1375</v>
+        <v>0.1236</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>0.0826</v>
+        <v>0.0719</v>
       </c>
       <c r="G19" s="4" t="n">
-        <v>0.0522</v>
+        <v>0.0619</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>0.1013</v>
+        <v>0.1001</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>0.0958</v>
+        <v>0.0882</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="4" t="n">
-        <v>0.0822</v>
+        <v>0.0638</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>0.0702</v>
+        <v>0.0647</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>0.0829</v>
+        <v>0.0867</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>0.1233</v>
+        <v>0.1385</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>0.069</v>
+        <v>0.0736</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>0.0609</v>
+        <v>0.0487</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>0.0999</v>
+        <v>0.1012</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>0.1041</v>
+        <v>0.0936</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="4" t="n">
-        <v>0.0996</v>
+        <v>0.0792</v>
       </c>
       <c r="C21" s="4" t="n">
-        <v>0.0769</v>
+        <v>0.0579</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>0.0854</v>
+        <v>0.0787</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>0.1266</v>
+        <v>0.1239</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>0.0786</v>
+        <v>0.0703</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>0.0737</v>
+        <v>0.0609</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>0.0846</v>
+        <v>0.1006</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>0.0996</v>
+        <v>0.1013</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="4" t="n">
-        <v>0.0916</v>
+        <v>0.0939</v>
       </c>
       <c r="C22" s="4" t="n">
-        <v>0.08</v>
+        <v>0.0725</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>0.0854</v>
+        <v>0.078</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>0.1266</v>
+        <v>0.1287</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>0.0766</v>
+        <v>0.0717</v>
       </c>
       <c r="G22" s="4" t="n">
-        <v>0.0671</v>
+        <v>0.0713</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>0.1017</v>
+        <v>0.085</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>0.1017</v>
+        <v>0.0953</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>0.0931</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>0.0752</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="E23" s="4" t="n">
+        <v>0.1138</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>0.0783</v>
+      </c>
+      <c r="G23" s="4" t="n">
+        <v>0.0727</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>0.1012</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <v>0.0987</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>0.0925</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>0.0846</v>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>0.0861</v>
+      </c>
+      <c r="E24" s="4" t="n">
+        <v>0.1326</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>0.0807</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <v>0.0545</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>0.0971</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <v>0.1213</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>0.0742</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>0.0784</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>0.0826</v>
+      </c>
+      <c r="E25" s="4" t="n">
+        <v>0.1315</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <v>0.0872</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <v>0.0674</v>
+      </c>
+      <c r="H25" s="4" t="n">
+        <v>0.0874</v>
+      </c>
+      <c r="I25" s="4" t="n">
+        <v>0.0964</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="7" t="n">
-        <f aca="false">AVERAGE(B16:B25)</f>
-        <v>0.0860142857142857</v>
-      </c>
-      <c r="C26" s="7" t="n">
-        <f aca="false">AVERAGE(C16:C25)</f>
-        <v>0.0736571428571429</v>
-      </c>
-      <c r="D26" s="7" t="n">
-        <f aca="false">AVERAGE(D16:D25)</f>
-        <v>0.0867142857142857</v>
-      </c>
-      <c r="E26" s="7" t="n">
-        <f aca="false">AVERAGE(E16:E25)</f>
-        <v>0.124371428571429</v>
-      </c>
-      <c r="F26" s="7" t="n">
-        <f aca="false">AVERAGE(F16:F25)</f>
-        <v>0.0759</v>
-      </c>
-      <c r="G26" s="7" t="n">
-        <f aca="false">AVERAGE(G16:G25)</f>
-        <v>0.067</v>
-      </c>
-      <c r="H26" s="7" t="n">
-        <f aca="false">AVERAGE(H16:H25)</f>
-        <v>0.0979428571428571</v>
-      </c>
-      <c r="I26" s="7" t="n">
-        <f aca="false">AVERAGE(I16:I25)</f>
-        <v>0.0968285714285714</v>
-      </c>
-      <c r="K26" s="7" t="n">
-        <f aca="false">AVERAGE(B26:I26)</f>
-        <v>0.0885535714285714</v>
+      <c r="B26" s="4" t="n">
+        <v>0.0647</v>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>0.085</v>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>0.0691</v>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>0.1187</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <v>0.0872</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>0.0821</v>
+      </c>
+      <c r="I26" s="4" t="n">
+        <v>0.0846</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8"/>
+      <c r="B27" s="7" t="n">
+        <f aca="false">AVERAGE(B17:B26)</f>
+        <v>0.0795</v>
+      </c>
+      <c r="C27" s="7" t="n">
+        <f aca="false">AVERAGE(C17:C26)</f>
+        <v>0.07238</v>
+      </c>
+      <c r="D27" s="7" t="n">
+        <f aca="false">AVERAGE(D17:D26)</f>
+        <v>0.08145</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <f aca="false">AVERAGE(E17:E26)</f>
+        <v>0.12455</v>
+      </c>
+      <c r="F27" s="7" t="n">
+        <f aca="false">AVERAGE(F17:F26)</f>
+        <v>0.07506</v>
+      </c>
+      <c r="G27" s="7" t="n">
+        <f aca="false">AVERAGE(G17:G26)</f>
+        <v>0.0649</v>
+      </c>
+      <c r="H27" s="7" t="n">
+        <f aca="false">AVERAGE(H17:H26)</f>
+        <v>0.09581</v>
+      </c>
+      <c r="I27" s="7" t="n">
+        <f aca="false">AVERAGE(I17:I26)</f>
+        <v>0.09624</v>
+      </c>
+      <c r="K27" s="7" t="n">
+        <f aca="false">AVERAGE(B27:I27)</f>
+        <v>0.08623625</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D14:G14"/>
+  <mergeCells count="2">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D15:G15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>